<commit_message>
Add tests for multiple sheets
</commit_message>
<xml_diff>
--- a/functions/test/lib/data.xlsx
+++ b/functions/test/lib/data.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId4"/>
+    <sheet name="BlahVtha" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Month</t>
   </si>
@@ -27,6 +28,18 @@
   </si>
   <si>
     <t>Sign ins per account</t>
+  </si>
+  <si>
+    <t>BLAH</t>
+  </si>
+  <si>
+    <t>VTHA</t>
+  </si>
+  <si>
+    <t>BTHA</t>
+  </si>
+  <si>
+    <t>VLAH</t>
   </si>
 </sst>
 </file>
@@ -60,7 +73,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,8 +98,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -286,13 +305,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -320,31 +429,52 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -370,6 +500,9 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1615,4 +1748,164 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="12" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="18" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="18" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="18" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="18" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="3">
+        <v>39963</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="6">
+        <v>39993</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7">
+        <v>22</v>
+      </c>
+      <c r="E3" s="8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="6">
+        <v>40024</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7">
+        <v>23</v>
+      </c>
+      <c r="E4" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="6">
+        <v>40055</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="6">
+        <v>40085</v>
+      </c>
+      <c r="B6" s="7">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" ht="14.65" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" ht="14.35" customHeight="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" ht="14.35" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" ht="14.35" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>